<commit_message>
added an excel file for report
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thesiliconpartner-my.sharepoint.com/personal/psingh3_tsp_tech/Documents/rpa/RE/RE-projectWithTabularData/Academic-REFTablular-UiDemo/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - The Silicon Partners Inc\rpa\RE\RE-projectWithTabularData\Academic-REFTablular-UiDemo\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16FDF2A4-535D-4A01-9335-14B56FB57A89}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5F9477-4595-4775-8058-FB27C3B9D462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -164,6 +164,12 @@
   </si>
   <si>
     <t>ManualTransactionThreshold</t>
+  </si>
+  <si>
+    <t>StatusFilePath</t>
+  </si>
+  <si>
+    <t>Data\Output\Status.xlsx</t>
   </si>
 </sst>
 </file>
@@ -541,7 +547,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -636,7 +642,14 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" t="s">
+        <v>48</v>
+      </c>
+    </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>

</xml_diff>